<commit_message>
[SIT] Big update page import with instruction import each feature.
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-account-user.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-account-user.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CF0CE6-11C3-42B0-8EFC-7D5764F53EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC544345-2A5F-40FE-A208-B4DEC2AFD146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="#account.users" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,9 +36,6 @@
     <t>STT</t>
   </si>
   <si>
-    <t>Tên đăng nhập (*)</t>
-  </si>
-  <si>
     <t>Họ (*)</t>
   </si>
   <si>
@@ -46,6 +43,9 @@
   </si>
   <si>
     <t>Mật khẩu (*)</t>
+  </si>
+  <si>
+    <t>Tên đăng nhập (*, định danh)</t>
   </si>
 </sst>
 </file>
@@ -424,13 +424,13 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.21875" customWidth="1"/>
     <col min="4" max="5" width="15.88671875" customWidth="1"/>
     <col min="6" max="6" width="36.6640625" customWidth="1"/>
@@ -442,16 +442,16 @@
         <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
[SIT] update view for import hr.
</commit_message>
<xml_diff>
--- a/apps/core/fimport/static/fimport/template/import-account-user.xlsx
+++ b/apps/core/fimport/static/fimport/template/import-account-user.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Coding\MIS\misui\apps\core\fimport\static\fimport\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC544345-2A5F-40FE-A208-B4DEC2AFD146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F557E8BB-5315-436C-B711-94D15562CB0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{ABCF866D-F0C2-489F-81F3-6B45D3E3629E}"/>
   </bookViews>
   <sheets>
     <sheet name="#account.users" sheetId="1" r:id="rId1"/>
+    <sheet name="Guidelines - Chỉ dẫn" sheetId="6" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="52">
   <si>
     <t>E-Mail</t>
   </si>
@@ -46,13 +47,310 @@
   </si>
   <si>
     <t>Tên đăng nhập (*, định danh)</t>
+  </si>
+  <si>
+    <t>Người dùng</t>
+  </si>
+  <si>
+    <t>Vai trò</t>
+  </si>
+  <si>
+    <t>Mô tả</t>
+  </si>
+  <si>
+    <t>#account.users</t>
+  </si>
+  <si>
+    <t>Tên sheet</t>
+  </si>
+  <si>
+    <t>Tên tính năng tiếng Anh</t>
+  </si>
+  <si>
+    <t>Tên tính năng tiếng Việt</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Mô tả thêm</t>
+  </si>
+  <si>
+    <t>Người dùng đăng nhập vào hệ thống</t>
+  </si>
+  <si>
+    <t>#hr.roles</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Vai trò của nhóm người dùng trong tổ chức (có cùng quyền hạn)</t>
+  </si>
+  <si>
+    <t>#hr.groups.level</t>
+  </si>
+  <si>
+    <t>Group Level</t>
+  </si>
+  <si>
+    <t>Cấp bậc nhóm</t>
+  </si>
+  <si>
+    <t>#hr.groups</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Nhóm</t>
+  </si>
+  <si>
+    <t>Các nhóm trong tổ chức - còn được gọi là phòng ban</t>
+  </si>
+  <si>
+    <t>Cấp bậc của các nhóm - còn được gọi là cấp bậc của phòng ban</t>
+  </si>
+  <si>
+    <t>#hr.employees</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Nhân viên</t>
+  </si>
+  <si>
+    <t>Nhân viên của công ty. Nếu nhân viên cho quyền đăng nhập vào hệ thống thì cung cấp #account.users và liên kết chúng với nhân viên.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phụ lục </t>
+  </si>
+  <si>
+    <t>Dữ liệu import</t>
+  </si>
+  <si>
+    <t>Ký hiệu</t>
+  </si>
+  <si>
+    <t>Bắt buộc</t>
+  </si>
+  <si>
+    <t>(*)</t>
+  </si>
+  <si>
+    <t>(*, định danh)</t>
+  </si>
+  <si>
+    <t>Bắt buộc và sử dụng dữ liệu này để định danh cho dòng dữ liệu này - sử dụng mã này ở các bảng liên kết tới nó</t>
+  </si>
+  <si>
+    <t>Là số thứ tự cho dòng dữ liệu. Sử dụng để xác định các dữ liệu đã được import,… luôn giữ cho chúng tăng dần để việc quản trị dữ liệu import của bạn dễ dàng hơn</t>
+  </si>
+  <si>
+    <t>Mô tả yêu cầu dữ liệu</t>
+  </si>
+  <si>
+    <t>Mô tả tên trang tính của từng tính năng</t>
+  </si>
+  <si>
+    <t>Mô tả tên trang tính</t>
+  </si>
+  <si>
+    <t>Số thứ tự</t>
+  </si>
+  <si>
+    <t>- Bắt buộc, định danh
+- Chuỗi định danh người dùng dùng để đăng nhập vào hệ thống
+- Chỉ chứa chữ cái, số, gạch ngang, gạch dưới
+- Ví dụ: anv</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Họ của người dùng
+- Ví dụ: Nguyễn Văn</t>
+  </si>
+  <si>
+    <t>- Bắt buộc
+- Tên của người dùng
+- Ví dụ: A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Bắt buộc
+- Mật khẩu truy cập của người dùng
+</t>
+  </si>
+  <si>
+    <t>- Địa chỉ thư điện tử của người dùng - sử dụng địa chỉ này để lấy lại mật khẩu.
+- Ví dụ: anv@example.com</t>
+  </si>
+  <si>
+    <t>- Số điện thoại của người dùng.
+- Định dạng số điện thoại ở VN
+- Ví dụ: 0987654321</t>
+  </si>
+  <si>
+    <t>Lưu ý</t>
+  </si>
+  <si>
+    <r>
+      <t>Khuyến cáo nên sử nhập dữ liệu</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Nhân viên</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> với các </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Nhóm</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> và </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Vai trò</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> có </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dữ liệu trống</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. 
+Sau đó sử dụng </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Mã nhân viên</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> cho các trường </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>thành viên của nhóm và vai trò</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Việc này nhân viên sẽ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tự động cập nhật các dữ liệu nhóm và vai trò liên kết</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,16 +366,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -100,15 +435,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -424,49 +825,373 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.88671875" customWidth="1"/>
-    <col min="2" max="2" width="27.88671875" customWidth="1"/>
-    <col min="3" max="3" width="19.21875" customWidth="1"/>
-    <col min="4" max="5" width="15.88671875" customWidth="1"/>
-    <col min="6" max="6" width="36.6640625" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="27.88671875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="19.21875" style="7" customWidth="1"/>
+    <col min="4" max="5" width="15.88671875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="36.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="22" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="str">
-        <f>IF(ISBLANK(B2), "", ROW(A2) -1)</f>
-        <v/>
+    <row r="2" spans="1:7" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B69A6E-98BC-434D-A419-FDB6C97F2A28}">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="28.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.6640625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="38.88671875" style="4" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="6"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="6"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="6"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="6"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="6"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="6"/>
+    </row>
+    <row r="16" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="13"/>
+      <c r="D17" s="13"/>
+      <c r="E17" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="1:5" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25"/>
+    </row>
+    <row r="26" spans="1:5" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B26" s="12"/>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+    </row>
+    <row r="27" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="2"/>
+    </row>
+    <row r="29" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" ht="62.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A16:E16"/>
+    <mergeCell ref="A26:E26"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B21:D21"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A3" location="'Instructions - Chỉ dẫn'!A26" display="Mô tả tên trang tính" xr:uid="{4E5C23A0-A79B-4E2E-B3C3-97237D68867F}"/>
+    <hyperlink ref="A2" location="'Instructions - Chỉ dẫn'!A16" display="Mô tả yêu cầu dữ liệu" xr:uid="{5511E882-0789-4D6F-AEAA-34360E5BE74D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>